<commit_message>
EPBDS-9201 make default  date format more preferable and add more tests
--HG--
branch : 5.22.x
</commit_message>
<xml_diff>
--- a/ITEST/itest.jacksonbinding/openl-repository/deployments/defaultdateformat/defaultdateformat.xlsx
+++ b/ITEST/itest.jacksonbinding/openl-repository/deployments/defaultdateformat/defaultdateformat.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-pub\ITEST\itest.jacksonbinding\openl-repository\deployments\defaultdateformat\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040DB96B-20AE-4B94-BB68-47C7FA795789}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19635" windowHeight="8190"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -14,18 +20,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Method Date getDate()</t>
   </si>
   <si>
     <t>return Date(2019,2,23);</t>
+  </si>
+  <si>
+    <t>Datatype DateWrapper</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>date1</t>
+  </si>
+  <si>
+    <t>date2</t>
+  </si>
+  <si>
+    <t>date3</t>
+  </si>
+  <si>
+    <t>date4</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>= dw</t>
+  </si>
+  <si>
+    <t>Spreadsheet DateWrapper spr(DateWrapper dw)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -73,13 +112,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -95,9 +138,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -135,9 +178,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -170,9 +213,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -205,9 +265,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -380,29 +457,91 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B5:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="39.140625" customWidth="1"/>
+    <col min="2" max="2" width="39.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B14:C14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-9201 Test dates for different timezones
</commit_message>
<xml_diff>
--- a/ITEST/itest.jacksonbinding/openl-repository/deployments/defaultdateformat/defaultdateformat.xlsx
+++ b/ITEST/itest.jacksonbinding/openl-repository/deployments/defaultdateformat/defaultdateformat.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-pub\ITEST\itest.jacksonbinding\openl-repository\deployments\defaultdateformat\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040DB96B-20AE-4B94-BB68-47C7FA795789}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Method Date getDate()</t>
   </si>
@@ -59,12 +53,15 @@
   </si>
   <si>
     <t>Spreadsheet DateWrapper spr(DateWrapper dw)</t>
+  </si>
+  <si>
+    <t>date5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -122,7 +119,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -138,9 +135,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -178,9 +175,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -213,26 +210,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -265,26 +245,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -457,35 +420,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="39.109375" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -493,7 +456,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -501,7 +464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -509,7 +472,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -517,12 +480,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>8</v>
       </c>
@@ -530,7 +501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>10</v>
       </c>

</xml_diff>